<commit_message>
Updating Old File for core commit 054f1d748c2d04cf17ed561d98a5746c15340109
</commit_message>
<xml_diff>
--- a/help/using/assets/CodeQuality-rules-latest-AMS.xlsx
+++ b/help/using/assets/CodeQuality-rules-latest-AMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedelson/OneDrive - Adobe Systems Incorporated/AMS/Pathlight/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/jedelson_adobe_com/Documents/AMS/Pathlight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA12BD1E-C8EE-BC4D-AAF0-24592B004DE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{3EBEEB8B-F071-664F-9C92-01DB5238DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AD697D3-8174-D342-BB66-FD2A0E285433}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="10140" windowWidth="38400" windowHeight="12000" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28080" windowHeight="17500" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="361">
   <si>
     <t>"@Deprecated" code should not be used</t>
   </si>
@@ -858,12 +858,6 @@
     <t>Product interfaces annotated with @ProviderType should not be implemented by custom code.</t>
   </si>
   <si>
-    <t>CQRules:CQBP-84--dependencies</t>
-  </si>
-  <si>
-    <t>Product interfaces annotated with @ProviderType should not be implemented in non-Adobe dependencies.</t>
-  </si>
-  <si>
     <t>BannedPaths</t>
   </si>
   <si>
@@ -1003,13 +997,124 @@
   </si>
   <si>
     <t>Custom Search Index Definition Nodes Must Not Contain a Property Named reindex</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-1---ignoreUrlParams-allow-list</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-2---statfileslevel</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-3---gracePeriod</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-4---default-filter-deny-rules</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-5---serveStaleOnError</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-6---suffix-allow-list</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-7---selector-allow-list</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-8---unique-farm-name</t>
+  </si>
+  <si>
+    <t>DOTRules:Httpd-1---require-all-granted</t>
+  </si>
+  <si>
+    <t>DOTRules:Syntax0---syntax-violation</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-S1---brace-missing</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-S2---token-unexpected</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-S3---quote-unmatched</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-S4---brace-unclosed</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-S5---mandatory-missing</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-S6---property-deprecated</t>
+  </si>
+  <si>
+    <t>DOTRules:Disp-S7---no-dispatcher-config</t>
+  </si>
+  <si>
+    <t>DOTRules:Httpd-S1---include-failed</t>
+  </si>
+  <si>
+    <t>beta,dispatcher</t>
+  </si>
+  <si>
+    <t>Each &lt;section name&gt; must begin with a '{' character.</t>
+  </si>
+  <si>
+    <t>Skipping unknown top level token.  Token="&lt;misplaced token&gt;"</t>
+  </si>
+  <si>
+    <t>Unmatched quote (").  Line="&lt;line details&gt;"</t>
+  </si>
+  <si>
+    <t>Unclosed brace encountered.</t>
+  </si>
+  <si>
+    <t>&lt;section name&gt; is missing mandatory '&lt;property name&gt;' value.</t>
+  </si>
+  <si>
+    <t>&lt;property name&gt; is deprecated.</t>
+  </si>
+  <si>
+    <t>Could not find Dispatcher configuration file.</t>
+  </si>
+  <si>
+    <t>Include directive must include existing files.  Check path, or use IncludeOptional.</t>
+  </si>
+  <si>
+    <t>Syntax issue encountered.</t>
+  </si>
+  <si>
+    <t>The Dispatcher publish farm cache should have its ignoreUrlParams rules configured in an allow list manner.</t>
+  </si>
+  <si>
+    <t>The Dispatcher publish farm cache statfileslevel property should be &gt;= 2.</t>
+  </si>
+  <si>
+    <t>The Dispatcher publish farm gracePeriod property should be &gt;= 2.</t>
+  </si>
+  <si>
+    <t>The Dispatcher publish farm filters should contain the default `deny` rules from the 6.x.x version of the AEM archetype.</t>
+  </si>
+  <si>
+    <t>The Dispatcher publish farm cache should have serveStaleOnError enabled.</t>
+  </si>
+  <si>
+    <t>The Dispatcher publish farm filters should specify the allowed Sling suffix patterns in an allow list manner.</t>
+  </si>
+  <si>
+    <t>The Dispatcher publish farm filters should specify the allowed Sling selectors in an allow list manner.</t>
+  </si>
+  <si>
+    <t>Each Dispatcher farm should have a unique name.</t>
+  </si>
+  <si>
+    <t>The 'Require all granted' directive should not be used in a VirtualHost Directory section with a root directory-path.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1033,6 +1138,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1055,10 +1173,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1374,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6A530D-317E-DF4C-BE2E-E97C27473266}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:J154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E129" sqref="A118:E129"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1969,10 +2089,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C35" t="s">
         <v>179</v>
@@ -2017,10 +2137,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B38" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C38" t="s">
         <v>179</v>
@@ -2028,16 +2148,13 @@
       <c r="D38" t="s">
         <v>159</v>
       </c>
-      <c r="E38" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>270</v>
+        <v>192</v>
       </c>
       <c r="B39" t="s">
-        <v>271</v>
+        <v>193</v>
       </c>
       <c r="C39" t="s">
         <v>179</v>
@@ -2045,13 +2162,16 @@
       <c r="D39" t="s">
         <v>159</v>
       </c>
+      <c r="E39" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C40" t="s">
         <v>179</v>
@@ -2065,10 +2185,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
         <v>179</v>
@@ -2077,15 +2197,15 @@
         <v>159</v>
       </c>
       <c r="E41" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
         <v>179</v>
@@ -2094,15 +2214,15 @@
         <v>159</v>
       </c>
       <c r="E42" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="C43" t="s">
         <v>179</v>
@@ -2111,32 +2231,32 @@
         <v>159</v>
       </c>
       <c r="E43" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>220</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>221</v>
       </c>
       <c r="C44" t="s">
         <v>179</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B45" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C45" t="s">
         <v>179</v>
@@ -2150,10 +2270,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B46" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C46" t="s">
         <v>179</v>
@@ -2167,10 +2287,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B47" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C47" t="s">
         <v>179</v>
@@ -2179,15 +2299,15 @@
         <v>171</v>
       </c>
       <c r="E47" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C48" t="s">
         <v>179</v>
@@ -2201,10 +2321,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="B49" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
       <c r="C49" t="s">
         <v>179</v>
@@ -2213,15 +2333,15 @@
         <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
         <v>179</v>
@@ -2230,15 +2350,15 @@
         <v>171</v>
       </c>
       <c r="E50" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
         <v>179</v>
@@ -2247,15 +2367,15 @@
         <v>171</v>
       </c>
       <c r="E51" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
         <v>179</v>
@@ -2264,15 +2384,15 @@
         <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
         <v>179</v>
@@ -2280,16 +2400,13 @@
       <c r="D53" t="s">
         <v>171</v>
       </c>
-      <c r="E53" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
         <v>179</v>
@@ -2297,13 +2414,16 @@
       <c r="D54" t="s">
         <v>171</v>
       </c>
+      <c r="E54" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
         <v>179</v>
@@ -2312,15 +2432,15 @@
         <v>171</v>
       </c>
       <c r="E55" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>206</v>
       </c>
       <c r="C56" t="s">
         <v>179</v>
@@ -2329,15 +2449,15 @@
         <v>171</v>
       </c>
       <c r="E56" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>205</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>206</v>
+        <v>23</v>
       </c>
       <c r="C57" t="s">
         <v>179</v>
@@ -2346,15 +2466,15 @@
         <v>171</v>
       </c>
       <c r="E57" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>195</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>196</v>
       </c>
       <c r="C58" t="s">
         <v>179</v>
@@ -2363,15 +2483,15 @@
         <v>171</v>
       </c>
       <c r="E58" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>195</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="C59" t="s">
         <v>179</v>
@@ -2380,15 +2500,15 @@
         <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>208</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>261</v>
       </c>
       <c r="C60" t="s">
         <v>179</v>
@@ -2397,15 +2517,15 @@
         <v>171</v>
       </c>
       <c r="E60" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>208</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>261</v>
+        <v>76</v>
       </c>
       <c r="C61" t="s">
         <v>179</v>
@@ -2414,15 +2534,15 @@
         <v>171</v>
       </c>
       <c r="E61" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="C62" t="s">
         <v>179</v>
@@ -2431,15 +2551,15 @@
         <v>171</v>
       </c>
       <c r="E62" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>204</v>
+        <v>259</v>
       </c>
       <c r="C63" t="s">
         <v>179</v>
@@ -2448,15 +2568,15 @@
         <v>171</v>
       </c>
       <c r="E63" t="s">
-        <v>184</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>210</v>
       </c>
       <c r="B64" t="s">
-        <v>259</v>
+        <v>211</v>
       </c>
       <c r="C64" t="s">
         <v>179</v>
@@ -2465,15 +2585,15 @@
         <v>171</v>
       </c>
       <c r="E64" t="s">
-        <v>260</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>86</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>87</v>
       </c>
       <c r="C65" t="s">
         <v>179</v>
@@ -2482,24 +2602,21 @@
         <v>171</v>
       </c>
       <c r="E65" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>279</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>280</v>
       </c>
       <c r="C66" t="s">
         <v>179</v>
       </c>
       <c r="D66" t="s">
         <v>171</v>
-      </c>
-      <c r="E66" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2532,24 +2649,27 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="B69" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="C69" t="s">
         <v>179</v>
       </c>
       <c r="D69" t="s">
-        <v>171</v>
+        <v>175</v>
+      </c>
+      <c r="E69" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>301</v>
+        <v>2</v>
       </c>
       <c r="C70" t="s">
         <v>179</v>
@@ -2558,15 +2678,15 @@
         <v>175</v>
       </c>
       <c r="E70" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="C71" t="s">
         <v>179</v>
@@ -2575,32 +2695,32 @@
         <v>175</v>
       </c>
       <c r="E71" t="s">
-        <v>177</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B72" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c r="D72" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="E72" t="s">
-        <v>262</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="C73" t="s">
         <v>226</v>
@@ -2609,15 +2729,15 @@
         <v>153</v>
       </c>
       <c r="E73" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>213</v>
       </c>
       <c r="B74" t="s">
-        <v>107</v>
+        <v>214</v>
       </c>
       <c r="C74" t="s">
         <v>226</v>
@@ -2626,32 +2746,32 @@
         <v>153</v>
       </c>
       <c r="E74" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>213</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="C75" t="s">
         <v>226</v>
       </c>
       <c r="D75" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E75" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>251</v>
+        <v>91</v>
       </c>
       <c r="C76" t="s">
         <v>226</v>
@@ -2665,10 +2785,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B77" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C77" t="s">
         <v>226</v>
@@ -2682,10 +2802,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="C78" t="s">
         <v>226</v>
@@ -2694,15 +2814,15 @@
         <v>159</v>
       </c>
       <c r="E78" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B79" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="C79" t="s">
         <v>226</v>
@@ -2711,15 +2831,15 @@
         <v>159</v>
       </c>
       <c r="E79" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B80" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C80" t="s">
         <v>226</v>
@@ -2728,15 +2848,15 @@
         <v>159</v>
       </c>
       <c r="E80" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="B81" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C81" t="s">
         <v>226</v>
@@ -2745,32 +2865,32 @@
         <v>159</v>
       </c>
       <c r="E81" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C82" t="s">
         <v>226</v>
       </c>
       <c r="D82" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="E82" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="C83" t="s">
         <v>226</v>
@@ -2779,15 +2899,15 @@
         <v>171</v>
       </c>
       <c r="E83" t="s">
-        <v>194</v>
+        <v>256</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>254</v>
+        <v>139</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="C84" t="s">
         <v>226</v>
@@ -2796,15 +2916,15 @@
         <v>171</v>
       </c>
       <c r="E84" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B85" t="s">
-        <v>229</v>
+        <v>24</v>
       </c>
       <c r="C85" t="s">
         <v>226</v>
@@ -2813,15 +2933,15 @@
         <v>171</v>
       </c>
       <c r="E85" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B86" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C86" t="s">
         <v>226</v>
@@ -2830,15 +2950,15 @@
         <v>171</v>
       </c>
       <c r="E86" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B87" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="C87" t="s">
         <v>226</v>
@@ -2847,15 +2967,15 @@
         <v>171</v>
       </c>
       <c r="E87" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B88" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C88" t="s">
         <v>226</v>
@@ -2864,15 +2984,15 @@
         <v>171</v>
       </c>
       <c r="E88" t="s">
-        <v>173</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="C89" t="s">
         <v>226</v>
@@ -2881,15 +3001,15 @@
         <v>171</v>
       </c>
       <c r="E89" t="s">
-        <v>252</v>
+        <v>203</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B90" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C90" t="s">
         <v>226</v>
@@ -2898,15 +3018,15 @@
         <v>171</v>
       </c>
       <c r="E90" t="s">
-        <v>203</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="B91" t="s">
-        <v>42</v>
+        <v>201</v>
       </c>
       <c r="C91" t="s">
         <v>226</v>
@@ -2915,15 +3035,15 @@
         <v>171</v>
       </c>
       <c r="E91" t="s">
-        <v>253</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="B92" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="C92" t="s">
         <v>226</v>
@@ -2932,15 +3052,15 @@
         <v>171</v>
       </c>
       <c r="E92" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>231</v>
+        <v>66</v>
       </c>
       <c r="B93" t="s">
-        <v>232</v>
+        <v>67</v>
       </c>
       <c r="C93" t="s">
         <v>226</v>
@@ -2949,15 +3069,15 @@
         <v>171</v>
       </c>
       <c r="E93" t="s">
-        <v>233</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B94" t="s">
-        <v>67</v>
+        <v>272</v>
       </c>
       <c r="C94" t="s">
         <v>226</v>
@@ -2966,15 +3086,15 @@
         <v>171</v>
       </c>
       <c r="E94" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>61</v>
+        <v>324</v>
       </c>
       <c r="B95" t="s">
-        <v>272</v>
+        <v>352</v>
       </c>
       <c r="C95" t="s">
         <v>226</v>
@@ -2983,305 +3103,305 @@
         <v>171</v>
       </c>
       <c r="E95" t="s">
-        <v>227</v>
+        <v>342</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>118</v>
+        <v>325</v>
       </c>
       <c r="B96" t="s">
-        <v>119</v>
+        <v>353</v>
       </c>
       <c r="C96" t="s">
         <v>226</v>
       </c>
       <c r="D96" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E96" t="s">
-        <v>194</v>
+        <v>342</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>124</v>
+        <v>326</v>
       </c>
       <c r="B97" t="s">
-        <v>125</v>
+        <v>354</v>
       </c>
       <c r="C97" t="s">
         <v>226</v>
       </c>
       <c r="D97" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E97" t="s">
-        <v>194</v>
+        <v>342</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>84</v>
+        <v>327</v>
       </c>
       <c r="B98" t="s">
-        <v>85</v>
+        <v>355</v>
       </c>
       <c r="C98" t="s">
         <v>226</v>
       </c>
       <c r="D98" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E98" t="s">
-        <v>250</v>
+        <v>342</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>120</v>
+        <v>328</v>
       </c>
       <c r="B99" t="s">
-        <v>121</v>
+        <v>356</v>
       </c>
       <c r="C99" t="s">
         <v>226</v>
       </c>
       <c r="D99" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E99" t="s">
-        <v>194</v>
+        <v>342</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>244</v>
+        <v>329</v>
       </c>
       <c r="B100" t="s">
-        <v>245</v>
+        <v>357</v>
       </c>
       <c r="C100" t="s">
         <v>226</v>
       </c>
       <c r="D100" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E100" t="s">
-        <v>230</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="B101" t="s">
-        <v>241</v>
+        <v>358</v>
       </c>
       <c r="C101" t="s">
         <v>226</v>
       </c>
       <c r="D101" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E101" t="s">
-        <v>230</v>
-      </c>
-      <c r="F101" s="2"/>
+        <v>342</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>236</v>
+        <v>331</v>
       </c>
       <c r="B102" t="s">
-        <v>237</v>
+        <v>359</v>
       </c>
       <c r="C102" t="s">
         <v>226</v>
       </c>
       <c r="D102" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E102" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>246</v>
+        <v>332</v>
       </c>
       <c r="B103" t="s">
-        <v>247</v>
+        <v>360</v>
       </c>
       <c r="C103" t="s">
         <v>226</v>
       </c>
       <c r="D103" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E103" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>273</v>
+        <v>333</v>
       </c>
       <c r="B104" t="s">
-        <v>274</v>
+        <v>351</v>
       </c>
       <c r="C104" t="s">
         <v>226</v>
       </c>
       <c r="D104" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E104" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>238</v>
+        <v>334</v>
       </c>
       <c r="B105" t="s">
-        <v>239</v>
+        <v>343</v>
       </c>
       <c r="C105" t="s">
         <v>226</v>
       </c>
       <c r="D105" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E105" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>234</v>
+        <v>335</v>
       </c>
       <c r="B106" t="s">
-        <v>235</v>
+        <v>344</v>
       </c>
       <c r="C106" t="s">
         <v>226</v>
       </c>
       <c r="D106" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E106" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>242</v>
+        <v>336</v>
       </c>
       <c r="B107" t="s">
-        <v>243</v>
+        <v>345</v>
       </c>
       <c r="C107" t="s">
         <v>226</v>
       </c>
       <c r="D107" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E107" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>248</v>
+        <v>337</v>
       </c>
       <c r="B108" t="s">
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="C108" t="s">
         <v>226</v>
       </c>
       <c r="D108" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E108" t="s">
-        <v>249</v>
+        <v>342</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>32</v>
+        <v>338</v>
       </c>
       <c r="B109" t="s">
-        <v>33</v>
+        <v>347</v>
       </c>
       <c r="C109" t="s">
         <v>226</v>
       </c>
       <c r="D109" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E109" t="s">
-        <v>257</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>81</v>
+        <v>339</v>
       </c>
       <c r="B110" t="s">
-        <v>258</v>
+        <v>348</v>
       </c>
       <c r="C110" t="s">
         <v>226</v>
       </c>
       <c r="D110" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E110" t="s">
-        <v>180</v>
+        <v>342</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>3</v>
+        <v>340</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>349</v>
       </c>
       <c r="C111" t="s">
         <v>226</v>
       </c>
       <c r="D111" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E111" t="s">
-        <v>198</v>
+        <v>342</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>287</v>
+        <v>341</v>
       </c>
       <c r="B112" t="s">
-        <v>299</v>
+        <v>350</v>
       </c>
       <c r="C112" t="s">
         <v>226</v>
       </c>
       <c r="D112" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E112" t="s">
-        <v>293</v>
+        <v>342</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>288</v>
+        <v>118</v>
       </c>
       <c r="B113" t="s">
-        <v>298</v>
+        <v>119</v>
       </c>
       <c r="C113" t="s">
         <v>226</v>
@@ -3290,15 +3410,15 @@
         <v>175</v>
       </c>
       <c r="E113" t="s">
-        <v>293</v>
+        <v>194</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>289</v>
+        <v>124</v>
       </c>
       <c r="B114" t="s">
-        <v>297</v>
+        <v>125</v>
       </c>
       <c r="C114" t="s">
         <v>226</v>
@@ -3307,15 +3427,15 @@
         <v>175</v>
       </c>
       <c r="E114" t="s">
-        <v>293</v>
+        <v>194</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>290</v>
+        <v>84</v>
       </c>
       <c r="B115" t="s">
-        <v>296</v>
+        <v>85</v>
       </c>
       <c r="C115" t="s">
         <v>226</v>
@@ -3324,15 +3444,15 @@
         <v>175</v>
       </c>
       <c r="E115" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>291</v>
+        <v>120</v>
       </c>
       <c r="B116" t="s">
-        <v>295</v>
+        <v>121</v>
       </c>
       <c r="C116" t="s">
         <v>226</v>
@@ -3341,15 +3461,15 @@
         <v>175</v>
       </c>
       <c r="E116" t="s">
-        <v>293</v>
+        <v>194</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
       <c r="B117" t="s">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="C117" t="s">
         <v>226</v>
@@ -3358,15 +3478,15 @@
         <v>175</v>
       </c>
       <c r="E117" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>302</v>
+        <v>240</v>
       </c>
       <c r="B118" t="s">
-        <v>303</v>
+        <v>241</v>
       </c>
       <c r="C118" t="s">
         <v>226</v>
@@ -3375,15 +3495,15 @@
         <v>175</v>
       </c>
       <c r="E118" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>304</v>
+        <v>236</v>
       </c>
       <c r="B119" t="s">
-        <v>315</v>
+        <v>237</v>
       </c>
       <c r="C119" t="s">
         <v>226</v>
@@ -3392,15 +3512,15 @@
         <v>175</v>
       </c>
       <c r="E119" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>305</v>
+        <v>246</v>
       </c>
       <c r="B120" t="s">
-        <v>316</v>
+        <v>247</v>
       </c>
       <c r="C120" t="s">
         <v>226</v>
@@ -3409,15 +3529,15 @@
         <v>175</v>
       </c>
       <c r="E120" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
       <c r="B121" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="C121" t="s">
         <v>226</v>
@@ -3426,15 +3546,15 @@
         <v>175</v>
       </c>
       <c r="E121" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>307</v>
+        <v>238</v>
       </c>
       <c r="B122" t="s">
-        <v>318</v>
+        <v>239</v>
       </c>
       <c r="C122" t="s">
         <v>226</v>
@@ -3443,15 +3563,15 @@
         <v>175</v>
       </c>
       <c r="E122" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>308</v>
+        <v>234</v>
       </c>
       <c r="B123" t="s">
-        <v>319</v>
+        <v>235</v>
       </c>
       <c r="C123" t="s">
         <v>226</v>
@@ -3460,15 +3580,15 @@
         <v>175</v>
       </c>
       <c r="E123" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>309</v>
+        <v>242</v>
       </c>
       <c r="B124" t="s">
-        <v>320</v>
+        <v>243</v>
       </c>
       <c r="C124" t="s">
         <v>226</v>
@@ -3477,15 +3597,15 @@
         <v>175</v>
       </c>
       <c r="E124" t="s">
-        <v>293</v>
+        <v>230</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>310</v>
+        <v>248</v>
       </c>
       <c r="B125" t="s">
-        <v>321</v>
+        <v>0</v>
       </c>
       <c r="C125" t="s">
         <v>226</v>
@@ -3494,15 +3614,15 @@
         <v>175</v>
       </c>
       <c r="E125" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>311</v>
+        <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>322</v>
+        <v>33</v>
       </c>
       <c r="C126" t="s">
         <v>226</v>
@@ -3511,15 +3631,15 @@
         <v>175</v>
       </c>
       <c r="E126" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>312</v>
+        <v>81</v>
       </c>
       <c r="B127" t="s">
-        <v>323</v>
+        <v>258</v>
       </c>
       <c r="C127" t="s">
         <v>226</v>
@@ -3528,76 +3648,434 @@
         <v>175</v>
       </c>
       <c r="E127" t="s">
-        <v>293</v>
+        <v>180</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" t="s">
+        <v>226</v>
+      </c>
+      <c r="D128" t="s">
+        <v>175</v>
+      </c>
+      <c r="E128" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>285</v>
+      </c>
+      <c r="B129" t="s">
+        <v>297</v>
+      </c>
+      <c r="C129" t="s">
+        <v>226</v>
+      </c>
+      <c r="D129" t="s">
+        <v>175</v>
+      </c>
+      <c r="E129" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>286</v>
+      </c>
+      <c r="B130" t="s">
+        <v>296</v>
+      </c>
+      <c r="C130" t="s">
+        <v>226</v>
+      </c>
+      <c r="D130" t="s">
+        <v>175</v>
+      </c>
+      <c r="E130" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>287</v>
+      </c>
+      <c r="B131" t="s">
+        <v>295</v>
+      </c>
+      <c r="C131" t="s">
+        <v>226</v>
+      </c>
+      <c r="D131" t="s">
+        <v>175</v>
+      </c>
+      <c r="E131" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>288</v>
+      </c>
+      <c r="B132" t="s">
+        <v>294</v>
+      </c>
+      <c r="C132" t="s">
+        <v>226</v>
+      </c>
+      <c r="D132" t="s">
+        <v>175</v>
+      </c>
+      <c r="E132" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>289</v>
+      </c>
+      <c r="B133" t="s">
+        <v>293</v>
+      </c>
+      <c r="C133" t="s">
+        <v>226</v>
+      </c>
+      <c r="D133" t="s">
+        <v>175</v>
+      </c>
+      <c r="E133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>290</v>
+      </c>
+      <c r="B134" t="s">
+        <v>292</v>
+      </c>
+      <c r="C134" t="s">
+        <v>226</v>
+      </c>
+      <c r="D134" t="s">
+        <v>175</v>
+      </c>
+      <c r="E134" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>300</v>
+      </c>
+      <c r="B135" t="s">
+        <v>301</v>
+      </c>
+      <c r="C135" t="s">
+        <v>226</v>
+      </c>
+      <c r="D135" t="s">
+        <v>175</v>
+      </c>
+      <c r="E135" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>302</v>
+      </c>
+      <c r="B136" t="s">
         <v>313</v>
       </c>
-      <c r="B128" t="s">
-        <v>324</v>
-      </c>
-      <c r="C128" t="s">
-        <v>226</v>
-      </c>
-      <c r="D128" t="s">
-        <v>175</v>
-      </c>
-      <c r="E128" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="C136" t="s">
+        <v>226</v>
+      </c>
+      <c r="D136" t="s">
+        <v>175</v>
+      </c>
+      <c r="E136" t="s">
+        <v>291</v>
+      </c>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="3"/>
+    </row>
+    <row r="137" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>303</v>
+      </c>
+      <c r="B137" t="s">
         <v>314</v>
       </c>
-      <c r="B129" t="s">
-        <v>325</v>
-      </c>
-      <c r="C129" t="s">
-        <v>226</v>
-      </c>
-      <c r="D129" t="s">
-        <v>175</v>
-      </c>
-      <c r="E129" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="C137" t="s">
+        <v>226</v>
+      </c>
+      <c r="D137" t="s">
+        <v>175</v>
+      </c>
+      <c r="E137" t="s">
+        <v>291</v>
+      </c>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+      <c r="J137" s="2"/>
+    </row>
+    <row r="138" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>304</v>
+      </c>
+      <c r="B138" t="s">
+        <v>315</v>
+      </c>
+      <c r="C138" t="s">
+        <v>226</v>
+      </c>
+      <c r="D138" t="s">
+        <v>175</v>
+      </c>
+      <c r="E138" t="s">
+        <v>291</v>
+      </c>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
+      <c r="J138" s="2"/>
+    </row>
+    <row r="139" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>305</v>
+      </c>
+      <c r="B139" t="s">
+        <v>316</v>
+      </c>
+      <c r="C139" t="s">
+        <v>226</v>
+      </c>
+      <c r="D139" t="s">
+        <v>175</v>
+      </c>
+      <c r="E139" t="s">
+        <v>291</v>
+      </c>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+      <c r="J139" s="2"/>
+    </row>
+    <row r="140" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>306</v>
+      </c>
+      <c r="B140" t="s">
+        <v>317</v>
+      </c>
+      <c r="C140" t="s">
+        <v>226</v>
+      </c>
+      <c r="D140" t="s">
+        <v>175</v>
+      </c>
+      <c r="E140" t="s">
+        <v>291</v>
+      </c>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="2"/>
+    </row>
+    <row r="141" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>307</v>
+      </c>
+      <c r="B141" t="s">
+        <v>318</v>
+      </c>
+      <c r="C141" t="s">
+        <v>226</v>
+      </c>
+      <c r="D141" t="s">
+        <v>175</v>
+      </c>
+      <c r="E141" t="s">
+        <v>291</v>
+      </c>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+      <c r="J141" s="2"/>
+    </row>
+    <row r="142" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>308</v>
+      </c>
+      <c r="B142" t="s">
+        <v>319</v>
+      </c>
+      <c r="C142" t="s">
+        <v>226</v>
+      </c>
+      <c r="D142" t="s">
+        <v>175</v>
+      </c>
+      <c r="E142" t="s">
+        <v>291</v>
+      </c>
+      <c r="H142" s="4"/>
+      <c r="I142" s="4"/>
+      <c r="J142" s="2"/>
+    </row>
+    <row r="143" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>309</v>
+      </c>
+      <c r="B143" t="s">
+        <v>320</v>
+      </c>
+      <c r="C143" t="s">
+        <v>226</v>
+      </c>
+      <c r="D143" t="s">
+        <v>175</v>
+      </c>
+      <c r="E143" t="s">
+        <v>291</v>
+      </c>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+      <c r="J143" s="2"/>
+    </row>
+    <row r="144" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>310</v>
+      </c>
+      <c r="B144" t="s">
+        <v>321</v>
+      </c>
+      <c r="C144" t="s">
+        <v>226</v>
+      </c>
+      <c r="D144" t="s">
+        <v>175</v>
+      </c>
+      <c r="E144" t="s">
+        <v>291</v>
+      </c>
+      <c r="H144" s="4"/>
+      <c r="I144" s="4"/>
+      <c r="J144" s="2"/>
+    </row>
+    <row r="145" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>311</v>
+      </c>
+      <c r="B145" t="s">
+        <v>322</v>
+      </c>
+      <c r="C145" t="s">
+        <v>226</v>
+      </c>
+      <c r="D145" t="s">
+        <v>175</v>
+      </c>
+      <c r="E145" t="s">
+        <v>291</v>
+      </c>
+      <c r="H145" s="4"/>
+      <c r="I145" s="4"/>
+      <c r="J145" s="2"/>
+    </row>
+    <row r="146" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>312</v>
+      </c>
+      <c r="B146" t="s">
+        <v>323</v>
+      </c>
+      <c r="C146" t="s">
+        <v>226</v>
+      </c>
+      <c r="D146" t="s">
+        <v>175</v>
+      </c>
+      <c r="E146" t="s">
+        <v>291</v>
+      </c>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="2"/>
+    </row>
+    <row r="147" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>134</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B147" t="s">
         <v>135</v>
       </c>
-      <c r="C130" t="s">
-        <v>226</v>
-      </c>
-      <c r="D130" t="s">
+      <c r="C147" t="s">
+        <v>226</v>
+      </c>
+      <c r="D147" t="s">
         <v>167</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E147" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="H147" s="4"/>
+      <c r="I147" s="4"/>
+      <c r="J147" s="2"/>
+    </row>
+    <row r="148" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>116</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B148" t="s">
         <v>117</v>
       </c>
-      <c r="C131" t="s">
-        <v>226</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="C148" t="s">
+        <v>226</v>
+      </c>
+      <c r="D148" t="s">
         <v>167</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E148" t="s">
         <v>173</v>
       </c>
+      <c r="H148" s="4"/>
+      <c r="I148" s="4"/>
+      <c r="J148" s="2"/>
+    </row>
+    <row r="149" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="H149" s="4"/>
+      <c r="I149" s="4"/>
+      <c r="J149" s="2"/>
+    </row>
+    <row r="150" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="H150" s="4"/>
+      <c r="I150" s="4"/>
+      <c r="J150" s="2"/>
+    </row>
+    <row r="151" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="H151" s="4"/>
+      <c r="I151" s="4"/>
+      <c r="J151" s="2"/>
+    </row>
+    <row r="152" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="H152" s="4"/>
+      <c r="I152" s="4"/>
+      <c r="J152" s="2"/>
+    </row>
+    <row r="153" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="H153" s="4"/>
+      <c r="I153" s="4"/>
+      <c r="J153" s="2"/>
+    </row>
+    <row r="154" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="H154" s="4"/>
+      <c r="I154" s="4"/>
+      <c r="J154" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Synced non localizable files from repo .
</commit_message>
<xml_diff>
--- a/help/using/assets/CodeQuality-rules-latest-AMS.xlsx
+++ b/help/using/assets/CodeQuality-rules-latest-AMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/jedelson_adobe_com/Documents/AMS/Pathlight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3EBEEB8B-F071-664F-9C92-01DB5238DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AD697D3-8174-D342-BB66-FD2A0E285433}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{3EBEEB8B-F071-664F-9C92-01DB5238DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50B1A3BB-9993-714B-9069-73DE8F09550A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28080" windowHeight="17500" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28060" windowHeight="17500" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="2" r:id="rId1"/>
@@ -858,9 +858,6 @@
     <t>Product interfaces annotated with @ProviderType should not be implemented by custom code.</t>
   </si>
   <si>
-    <t>BannedPaths</t>
-  </si>
-  <si>
     <t>Customer packages should not install content under /libs</t>
   </si>
   <si>
@@ -1108,6 +1105,9 @@
   </si>
   <si>
     <t>The 'Require all granted' directive should not be used in a VirtualHost Directory section with a root directory-path.</t>
+  </si>
+  <si>
+    <t>BannedPath</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1497,7 @@
   <dimension ref="A1:J154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>360</v>
+      </c>
+      <c r="B35" t="s">
         <v>277</v>
-      </c>
-      <c r="B35" t="s">
-        <v>278</v>
       </c>
       <c r="C35" t="s">
         <v>179</v>
@@ -2607,10 +2607,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>278</v>
+      </c>
+      <c r="B66" t="s">
         <v>279</v>
-      </c>
-      <c r="B66" t="s">
-        <v>280</v>
       </c>
       <c r="C66" t="s">
         <v>179</v>
@@ -2621,10 +2621,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>280</v>
+      </c>
+      <c r="B67" t="s">
         <v>281</v>
-      </c>
-      <c r="B67" t="s">
-        <v>282</v>
       </c>
       <c r="C67" t="s">
         <v>179</v>
@@ -2635,10 +2635,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>282</v>
+      </c>
+      <c r="B68" t="s">
         <v>283</v>
-      </c>
-      <c r="B68" t="s">
-        <v>284</v>
       </c>
       <c r="C68" t="s">
         <v>179</v>
@@ -2649,10 +2649,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>297</v>
+      </c>
+      <c r="B69" t="s">
         <v>298</v>
-      </c>
-      <c r="B69" t="s">
-        <v>299</v>
       </c>
       <c r="C69" t="s">
         <v>179</v>
@@ -3091,10 +3091,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B95" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C95" t="s">
         <v>226</v>
@@ -3103,15 +3103,15 @@
         <v>171</v>
       </c>
       <c r="E95" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B96" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C96" t="s">
         <v>226</v>
@@ -3120,15 +3120,15 @@
         <v>171</v>
       </c>
       <c r="E96" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B97" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C97" t="s">
         <v>226</v>
@@ -3137,15 +3137,15 @@
         <v>171</v>
       </c>
       <c r="E97" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B98" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C98" t="s">
         <v>226</v>
@@ -3154,15 +3154,15 @@
         <v>171</v>
       </c>
       <c r="E98" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B99" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C99" t="s">
         <v>226</v>
@@ -3171,15 +3171,15 @@
         <v>171</v>
       </c>
       <c r="E99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B100" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C100" t="s">
         <v>226</v>
@@ -3188,16 +3188,16 @@
         <v>171</v>
       </c>
       <c r="E100" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B101" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C101" t="s">
         <v>226</v>
@@ -3206,15 +3206,15 @@
         <v>171</v>
       </c>
       <c r="E101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C102" t="s">
         <v>226</v>
@@ -3223,15 +3223,15 @@
         <v>171</v>
       </c>
       <c r="E102" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B103" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C103" t="s">
         <v>226</v>
@@ -3240,15 +3240,15 @@
         <v>171</v>
       </c>
       <c r="E103" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B104" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C104" t="s">
         <v>226</v>
@@ -3257,15 +3257,15 @@
         <v>171</v>
       </c>
       <c r="E104" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B105" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C105" t="s">
         <v>226</v>
@@ -3274,15 +3274,15 @@
         <v>171</v>
       </c>
       <c r="E105" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B106" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C106" t="s">
         <v>226</v>
@@ -3291,15 +3291,15 @@
         <v>171</v>
       </c>
       <c r="E106" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B107" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C107" t="s">
         <v>226</v>
@@ -3308,15 +3308,15 @@
         <v>171</v>
       </c>
       <c r="E107" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B108" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C108" t="s">
         <v>226</v>
@@ -3325,15 +3325,15 @@
         <v>171</v>
       </c>
       <c r="E108" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B109" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C109" t="s">
         <v>226</v>
@@ -3342,15 +3342,15 @@
         <v>171</v>
       </c>
       <c r="E109" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B110" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C110" t="s">
         <v>226</v>
@@ -3359,15 +3359,15 @@
         <v>171</v>
       </c>
       <c r="E110" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B111" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C111" t="s">
         <v>226</v>
@@ -3376,24 +3376,24 @@
         <v>171</v>
       </c>
       <c r="E111" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>340</v>
+      </c>
+      <c r="B112" t="s">
+        <v>349</v>
+      </c>
+      <c r="C112" t="s">
+        <v>226</v>
+      </c>
+      <c r="D112" t="s">
+        <v>171</v>
+      </c>
+      <c r="E112" t="s">
         <v>341</v>
-      </c>
-      <c r="B112" t="s">
-        <v>350</v>
-      </c>
-      <c r="C112" t="s">
-        <v>226</v>
-      </c>
-      <c r="D112" t="s">
-        <v>171</v>
-      </c>
-      <c r="E112" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -3670,10 +3670,10 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B129" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C129" t="s">
         <v>226</v>
@@ -3682,15 +3682,15 @@
         <v>175</v>
       </c>
       <c r="E129" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B130" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C130" t="s">
         <v>226</v>
@@ -3699,15 +3699,15 @@
         <v>175</v>
       </c>
       <c r="E130" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B131" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C131" t="s">
         <v>226</v>
@@ -3716,15 +3716,15 @@
         <v>175</v>
       </c>
       <c r="E131" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C132" t="s">
         <v>226</v>
@@ -3733,15 +3733,15 @@
         <v>175</v>
       </c>
       <c r="E132" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B133" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C133" t="s">
         <v>226</v>
@@ -3750,33 +3750,33 @@
         <v>175</v>
       </c>
       <c r="E133" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>289</v>
+      </c>
+      <c r="B134" t="s">
+        <v>291</v>
+      </c>
+      <c r="C134" t="s">
+        <v>226</v>
+      </c>
+      <c r="D134" t="s">
+        <v>175</v>
+      </c>
+      <c r="E134" t="s">
         <v>290</v>
-      </c>
-      <c r="B134" t="s">
-        <v>292</v>
-      </c>
-      <c r="C134" t="s">
-        <v>226</v>
-      </c>
-      <c r="D134" t="s">
-        <v>175</v>
-      </c>
-      <c r="E134" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>299</v>
+      </c>
+      <c r="B135" t="s">
         <v>300</v>
       </c>
-      <c r="B135" t="s">
-        <v>301</v>
-      </c>
       <c r="C135" t="s">
         <v>226</v>
       </c>
@@ -3784,15 +3784,15 @@
         <v>175</v>
       </c>
       <c r="E135" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B136" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C136" t="s">
         <v>226</v>
@@ -3801,7 +3801,7 @@
         <v>175</v>
       </c>
       <c r="E136" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -3809,10 +3809,10 @@
     </row>
     <row r="137" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B137" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C137" t="s">
         <v>226</v>
@@ -3821,7 +3821,7 @@
         <v>175</v>
       </c>
       <c r="E137" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
@@ -3829,10 +3829,10 @@
     </row>
     <row r="138" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B138" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C138" t="s">
         <v>226</v>
@@ -3841,7 +3841,7 @@
         <v>175</v>
       </c>
       <c r="E138" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
@@ -3849,10 +3849,10 @@
     </row>
     <row r="139" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B139" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C139" t="s">
         <v>226</v>
@@ -3861,7 +3861,7 @@
         <v>175</v>
       </c>
       <c r="E139" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
@@ -3869,10 +3869,10 @@
     </row>
     <row r="140" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B140" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C140" t="s">
         <v>226</v>
@@ -3881,7 +3881,7 @@
         <v>175</v>
       </c>
       <c r="E140" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -3889,10 +3889,10 @@
     </row>
     <row r="141" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B141" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C141" t="s">
         <v>226</v>
@@ -3901,7 +3901,7 @@
         <v>175</v>
       </c>
       <c r="E141" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -3909,10 +3909,10 @@
     </row>
     <row r="142" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B142" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C142" t="s">
         <v>226</v>
@@ -3921,7 +3921,7 @@
         <v>175</v>
       </c>
       <c r="E142" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -3929,10 +3929,10 @@
     </row>
     <row r="143" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B143" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C143" t="s">
         <v>226</v>
@@ -3941,7 +3941,7 @@
         <v>175</v>
       </c>
       <c r="E143" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -3949,10 +3949,10 @@
     </row>
     <row r="144" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B144" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C144" t="s">
         <v>226</v>
@@ -3961,7 +3961,7 @@
         <v>175</v>
       </c>
       <c r="E144" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -3969,10 +3969,10 @@
     </row>
     <row r="145" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B145" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C145" t="s">
         <v>226</v>
@@ -3981,7 +3981,7 @@
         <v>175</v>
       </c>
       <c r="E145" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -3989,10 +3989,10 @@
     </row>
     <row r="146" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C146" t="s">
         <v>226</v>
@@ -4001,7 +4001,7 @@
         <v>175</v>
       </c>
       <c r="E146" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>

</xml_diff>